<commit_message>
Entrega de documentación - Segundo Corte.
</commit_message>
<xml_diff>
--- a/Bitácora/BITACORA GOPOLI.xlsx
+++ b/Bitácora/BITACORA GOPOLI.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22820"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_34ce\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3671\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00956B86-DC0E-4004-9D8A-BC5CC6768BFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A223572F-49B1-49AA-A196-75A4247C3BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitácora General" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Bitácora General'!$F$4:$F$30</definedName>
+  </definedNames>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
   <si>
     <t>PROYECTO GOPOLI (Bitácora)</t>
   </si>
@@ -122,6 +125,12 @@
     <t>Se planeo una reunion con el grupo de trabajo de ingenieria de sistemas para ajustar los horarios de trabajos una vez sean enregados los mockups por parte de los diseñadores.</t>
   </si>
   <si>
+    <t>1:30 Hr</t>
+  </si>
+  <si>
+    <t>Sebastian Felipe Moreno Gómez</t>
+  </si>
+  <si>
     <t>Trabajo</t>
   </si>
   <si>
@@ -134,9 +143,6 @@
     <t>Realice una aplicación que consistia en una calculadora, la cual era la mejora de aquella que habiamos iniciado en clase. Esta vez la aplicacion conteneria las operaciones de resta, multiplicacion, division y valor absoluto ademas de la operacion suma que fue la realizada en clase</t>
   </si>
   <si>
-    <t>Sebastian Felipe Moreno Gómez</t>
-  </si>
-  <si>
     <t>Desarrollo de aplicación Tic Tac Toe</t>
   </si>
   <si>
@@ -164,13 +170,79 @@
     <t>Videos tutoriales de bases de datos</t>
   </si>
   <si>
+    <t>Lunes, 23 de Marzo</t>
+  </si>
+  <si>
+    <t>Videos enviados por Paul, lider del grupo de ingenieros, para aprender sobre bases de datos, videos los cuales son necesarios para el desarrollo de aplicaciones.</t>
+  </si>
+  <si>
+    <t>Llenado de bitacora</t>
+  </si>
+  <si>
     <t>EN PROCESO</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Videos enviados por Paul, lider del grupo de ingenieros, para aprender sobre bases de datos, videos los cuales son necesarios para el desarrollo de aplicaciones.</t>
+    <t>Miercoles, 4 de Marzo</t>
+  </si>
+  <si>
+    <t>Se realiza el llenado de la bitacora para mantener todas la actividades organizadas</t>
+  </si>
+  <si>
+    <t>Complementación de Requisitos de la app</t>
+  </si>
+  <si>
+    <t>3:00 Hr</t>
+  </si>
+  <si>
+    <t>Viernes, 6 de Marzo</t>
+  </si>
+  <si>
+    <t>Se realizo la complementación del documento sobre los requisitos que necesita la aplicación para funcionar correctamente</t>
+  </si>
+  <si>
+    <t>Martes, 10 de Marzo</t>
+  </si>
+  <si>
+    <t>Realice una aplicación que consistia manejar dos textos y tener el poder de sumarlos, multiplicarlos, dividirlos o restarlos. Utilizando los conocimientos adqueridos en videos de Java.</t>
+  </si>
+  <si>
+    <t>Diana Sofia Pulido Gomez</t>
+  </si>
+  <si>
+    <t>5:00 Hr</t>
+  </si>
+  <si>
+    <t>2:00 Hr</t>
+  </si>
+  <si>
+    <t>Curso Bases de Datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vi todos los videos asignados por el lider Kevin Montealegre el cual era guiado hacia el aprendizaje de la creación y manejo de datos. Esta tarea serviría para la base de datos de la aplicación </t>
+  </si>
+  <si>
+    <t>Diseño Base de Datos</t>
+  </si>
+  <si>
+    <t>12:00 Hr</t>
+  </si>
+  <si>
+    <t>Lunes, 31 de Marzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se realizo la base de datos de la aplicación en la plataforma MySQL. De las 12 horas nos tomo 10 la elaboración y 2 horas planeación </t>
+  </si>
+  <si>
+    <t>Desarrollo en Android Studio</t>
+  </si>
+  <si>
+    <t>5 Dias</t>
+  </si>
+  <si>
+    <t>Miercoles, 22 de Abril</t>
+  </si>
+  <si>
+    <t>Se realizo la implementación de Actividades y el Servicio en Android del Sensor de Pasos</t>
   </si>
 </sst>
 </file>
@@ -239,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -278,17 +350,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -330,15 +391,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -402,56 +454,29 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -461,34 +486,23 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -498,142 +512,89 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -916,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="D24" zoomScale="141" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -928,7 +889,7 @@
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
@@ -938,14 +899,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -957,55 +918,55 @@
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1">
       <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1">
-      <c r="A5" s="37"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="34"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="38"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="35"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:15" ht="72.95" customHeight="1">
       <c r="A7" s="8" t="s">
@@ -1040,7 +1001,7 @@
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1060,7 +1021,7 @@
       <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="13" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -1071,7 +1032,7 @@
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="7"/>
@@ -1103,159 +1064,376 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="102" customHeight="1">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:15" ht="90">
+      <c r="A12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:15" ht="102" customHeight="1">
+      <c r="A13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="101.25" customHeight="1">
+      <c r="A14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="75.75" customHeight="1">
+      <c r="A15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="75.75" customHeight="1">
+      <c r="A16" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="75.75" customHeight="1">
+      <c r="A17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="60">
+      <c r="A18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90">
+      <c r="A19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="C19" s="17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="101.25" customHeight="1">
-      <c r="A13" s="17" t="s">
+      <c r="D19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90">
+      <c r="A20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="D20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="63.75" customHeight="1">
+      <c r="A21" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60">
+      <c r="A22" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="105">
+      <c r="A23" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="135">
+      <c r="A24" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="18" t="s">
+      <c r="F24" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="90">
+      <c r="A25" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="75.75" customHeight="1">
-      <c r="A14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="75">
-      <c r="A15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="D25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="10"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="10"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="10"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="10"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="10"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="10"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="10"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
+      <c r="E25" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60">
+      <c r="A26" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60">
+      <c r="A27" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60">
+      <c r="A28" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45">
+      <c r="A29" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
     </row>
   </sheetData>
+  <autoFilter ref="F4:F30" xr:uid="{FD758C71-EFB1-4734-8EFA-6C79F7547643}"/>
   <mergeCells count="7">
     <mergeCell ref="A1:F3"/>
     <mergeCell ref="B4:B6"/>

</xml_diff>